<commit_message>
update excel file mle
</commit_message>
<xml_diff>
--- a/CodeTemplates/SlugsTemplate.xlsx
+++ b/CodeTemplates/SlugsTemplate.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfieberg\Documents\Teaching\Stats4EcologistsFiles\CodeTemplates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E407DC5-D3DB-48D4-A6A5-1ED0E3B2E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="15075"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slugs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,12 +585,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -636,6 +658,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCB9-45C3-814C-803DED08AF0D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -682,7 +709,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -714,7 +740,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -733,9 +765,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -773,7 +805,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -845,7 +877,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1018,20 +1050,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:E84"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1080,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1065,411 +1097,411 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <f>EXP(-B1)*B1^A3/FACT(A3)</f>
+        <f>EXP(-B$1)*B$1^$A3/FACT($A3)</f>
         <v>6.1313240195240391E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -1490,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>4</v>
       </c>

</xml_diff>